<commit_message>
Finalisation du tableaux d'analyses ( valeurs de références + débruitage par NN )
</commit_message>
<xml_diff>
--- a/code/DB/Tableau analyse.xlsx
+++ b/code/DB/Tableau analyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoli\OneDrive\Desktop\HAI927-Projet_IMAGE\code\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD87274-DE15-4917-B232-B24FDEC62F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330E6A2D-AAFE-4A1B-B299-FAE3F9D6FCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{72593B04-D0A3-4FED-B0AF-9F94CC81D14A}"/>
+    <workbookView xWindow="12528" yWindow="0" windowWidth="10608" windowHeight="8952" firstSheet="4" activeTab="4" xr2:uid="{72593B04-D0A3-4FED-B0AF-9F94CC81D14A}"/>
   </bookViews>
   <sheets>
     <sheet name="Best Param" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="96">
   <si>
     <t>Speckle</t>
   </si>
@@ -323,13 +323,19 @@
   </si>
   <si>
     <t>voisins = 1     puissance = 0.5</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +459,20 @@
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF009999"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,6 +676,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -665,83 +754,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,15 +771,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF009999"/>
       <color rgb="FF996600"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF339933"/>
       <color rgb="FFCC0000"/>
+      <color rgb="FF00CC99"/>
       <color rgb="FFCC9900"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF0033CC"/>
       <color rgb="FF9933FF"/>
-      <color rgb="FFFF9933"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1297,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B2F242-EB2C-4F2C-A6FA-93070B168A44}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="N3" zoomScale="79" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,351 +1332,459 @@
     <col min="33" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:22" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="25">
+      <c r="R4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="42"/>
+      <c r="C5" s="22">
         <v>2.5</v>
       </c>
       <c r="D5" s="17">
         <v>30.38</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="44" t="s">
         <v>56</v>
       </c>
       <c r="F5" s="17">
         <v>29.46</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="44" t="s">
         <v>42</v>
       </c>
       <c r="H5" s="17">
         <v>31.2</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>45</v>
       </c>
       <c r="J5" s="17">
         <v>29.87</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="44" t="s">
         <v>47</v>
       </c>
       <c r="L5" s="17">
         <v>41.78</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="45" t="s">
         <v>48</v>
       </c>
       <c r="N5" s="17">
         <v>39.94</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="32">
         <v>41.78</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="25">
+      <c r="R5" s="38">
+        <v>41.83</v>
+      </c>
+      <c r="T5" s="32">
+        <v>41.78</v>
+      </c>
+      <c r="U5" s="46">
+        <v>35.67</v>
+      </c>
+      <c r="V5" s="38">
+        <v>41.78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42"/>
+      <c r="C6" s="22">
         <v>5</v>
       </c>
       <c r="D6" s="17">
         <v>30.11</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="17">
         <v>29.02</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17">
         <v>30.64</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="17">
         <v>29.64</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="17">
         <v>34.200000000000003</v>
       </c>
-      <c r="M6" s="32"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="17">
         <v>34.49</v>
       </c>
-      <c r="O6" s="35"/>
-      <c r="Q6" s="39">
+      <c r="O6" s="40"/>
+      <c r="Q6" s="33">
         <v>34.39</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="25">
+      <c r="R6" s="38">
+        <v>34.21</v>
+      </c>
+      <c r="T6" s="33">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="U6" s="46">
+        <v>34.380000000000003</v>
+      </c>
+      <c r="V6" s="38">
+        <v>34.11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="42"/>
+      <c r="C7" s="22">
         <v>7.5</v>
       </c>
       <c r="D7" s="17">
         <v>29.86</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="17">
         <v>28.66</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="17">
         <v>30.15</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="17">
         <v>29.4</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="17">
         <v>31.31</v>
       </c>
-      <c r="M7" s="32"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="17">
         <v>32.950000000000003</v>
       </c>
-      <c r="O7" s="34" t="s">
+      <c r="O7" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="33">
         <v>32.950000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="25">
+      <c r="R7" s="38">
+        <v>31.33</v>
+      </c>
+      <c r="T7" s="33">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="U7" s="46">
+        <v>33.53</v>
+      </c>
+      <c r="V7" s="38">
+        <v>31.23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="22">
         <v>10</v>
       </c>
       <c r="D8" s="17">
         <v>29.38</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="17">
         <v>28.09</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="17">
         <v>29.37</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="17">
         <v>28.98</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="17">
         <v>28.3</v>
       </c>
-      <c r="M8" s="32"/>
+      <c r="M8" s="45"/>
       <c r="N8" s="17">
         <v>31.15</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="33">
         <v>31.15</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="25">
+      <c r="R8" s="38">
+        <v>28.3</v>
+      </c>
+      <c r="T8" s="33">
+        <v>33.229999999999997</v>
+      </c>
+      <c r="U8" s="46">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="V8" s="38">
+        <v>28.18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
+      <c r="C9" s="22">
         <v>15</v>
       </c>
       <c r="D9" s="17">
         <v>28.47</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="17">
         <v>27.02</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="17">
         <v>28.04</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="17">
         <v>28.15</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="17">
         <v>24.87</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="17">
         <v>29.17</v>
       </c>
-      <c r="O9" s="35" t="s">
+      <c r="O9" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="33">
         <v>29.17</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="25">
+      <c r="R9" s="38">
+        <v>24.87</v>
+      </c>
+      <c r="T9" s="33">
+        <v>30.35</v>
+      </c>
+      <c r="U9" s="46">
+        <v>30.32</v>
+      </c>
+      <c r="V9" s="38">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42"/>
+      <c r="C10" s="22">
         <v>20</v>
       </c>
       <c r="D10" s="17">
         <v>27.53</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="17">
         <v>25.93</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="17">
         <v>26.78</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="17">
         <v>27.27</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="17">
         <v>24.08</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="45" t="s">
         <v>64</v>
       </c>
       <c r="N10" s="17">
         <v>27.71</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="Q10" s="39">
+      <c r="O10" s="40"/>
+      <c r="Q10" s="33">
         <v>27.71</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="25">
+      <c r="R10" s="38">
+        <v>22.46</v>
+      </c>
+      <c r="T10" s="33">
+        <v>28.65</v>
+      </c>
+      <c r="U10" s="46">
+        <v>28.68</v>
+      </c>
+      <c r="V10" s="38">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42"/>
+      <c r="C11" s="22">
         <v>25</v>
       </c>
       <c r="D11" s="17">
         <v>26.6</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17">
         <v>24.88</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="17">
         <v>25.62</v>
       </c>
-      <c r="I11" s="32"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="17">
         <v>26.39</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="17">
         <v>23.64</v>
       </c>
-      <c r="M11" s="32"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="17">
         <v>26.4</v>
       </c>
-      <c r="O11" s="35"/>
-      <c r="Q11" s="40">
+      <c r="O11" s="40"/>
+      <c r="Q11" s="34">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20"/>
-      <c r="C12" s="25">
+      <c r="R11" s="38">
+        <v>20.61</v>
+      </c>
+      <c r="T11" s="34">
+        <v>27.93</v>
+      </c>
+      <c r="U11" s="46">
+        <v>27.25</v>
+      </c>
+      <c r="V11" s="38">
+        <v>20.420000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="22">
         <v>35</v>
       </c>
       <c r="D12" s="17">
         <v>24.88</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="17">
         <v>23.21</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H12" s="17">
         <v>24.28</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="17">
         <v>24.73</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="17">
         <v>22.64</v>
       </c>
-      <c r="M12" s="32"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="17">
         <v>24.42</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" s="40">
+      <c r="Q12" s="34">
         <v>24.88</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+      <c r="R12" s="38">
+        <v>17.89</v>
+      </c>
+      <c r="T12" s="34">
+        <v>25.85</v>
+      </c>
+      <c r="U12" s="46">
+        <v>24.75</v>
+      </c>
+      <c r="V12" s="38">
+        <v>17.66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="M13" s="29"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M14" s="29"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1670,15 +1799,16 @@
     <mergeCell ref="M10:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B74CB-B6B1-4D07-A0EC-CDD20D1CE1F8}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="M7" zoomScale="75" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,359 +1819,467 @@
     <col min="33" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:22" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="25">
+      <c r="R4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="42"/>
+      <c r="C5" s="22">
         <v>2.5</v>
       </c>
       <c r="D5" s="17">
         <v>29.33</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="44" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="17">
         <v>28.22</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="44" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="17">
         <v>31.2</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="17">
         <v>28.94</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="17">
         <v>29.02</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="44" t="s">
         <v>63</v>
       </c>
       <c r="N5" s="17">
         <v>34.380000000000003</v>
       </c>
-      <c r="O5" s="41" t="s">
+      <c r="O5" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="39">
+      <c r="Q5" s="33">
         <v>34.380000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="25">
+      <c r="R5" s="38">
+        <v>29.01</v>
+      </c>
+      <c r="T5" s="33">
+        <v>35.76</v>
+      </c>
+      <c r="U5" s="46">
+        <v>33.979999999999997</v>
+      </c>
+      <c r="V5" s="38">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42"/>
+      <c r="C6" s="22">
         <v>5</v>
       </c>
       <c r="D6" s="17">
         <v>27.94</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="17">
         <v>26.59</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17">
         <v>30.77</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="17">
         <v>27.65</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="17">
         <v>25.01</v>
       </c>
-      <c r="M6" s="32"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="17">
         <v>30.14</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="Q6" s="35">
         <v>30.77</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="25">
+      <c r="R6" s="38">
+        <v>25.03</v>
+      </c>
+      <c r="T6" s="35">
+        <v>32.9</v>
+      </c>
+      <c r="U6" s="46">
+        <v>32.21</v>
+      </c>
+      <c r="V6" s="38">
+        <v>26.17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="42"/>
+      <c r="C7" s="22">
         <v>7.5</v>
       </c>
       <c r="D7" s="17">
         <v>27.18</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="17">
         <v>25.67</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="17">
         <v>30.39</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="17">
         <v>26.88</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="17">
         <v>23.98</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="28" t="s">
         <v>65</v>
       </c>
       <c r="N7" s="17">
         <v>30</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="Q7" s="43">
+      <c r="O7" s="40"/>
+      <c r="Q7" s="35">
         <v>30.39</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="25">
+      <c r="R7" s="38">
+        <v>23.54</v>
+      </c>
+      <c r="T7" s="35">
+        <v>32.47</v>
+      </c>
+      <c r="U7" s="46">
+        <v>31.34</v>
+      </c>
+      <c r="V7" s="38">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="22">
         <v>10</v>
       </c>
       <c r="D8" s="17">
         <v>26</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="17">
         <v>24.48</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="17">
         <v>29.56</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="17">
         <v>25.8</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="17">
         <v>23.41</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="45" t="s">
         <v>66</v>
       </c>
       <c r="N8" s="17">
         <v>26.83</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="Q8" s="43">
+      <c r="O8" s="40"/>
+      <c r="Q8" s="35">
         <v>29.56</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="25">
+      <c r="R8" s="38">
+        <v>22.01</v>
+      </c>
+      <c r="T8" s="35">
+        <v>31.69</v>
+      </c>
+      <c r="U8" s="46">
+        <v>30.21</v>
+      </c>
+      <c r="V8" s="38">
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
+      <c r="C9" s="22">
         <v>15</v>
       </c>
       <c r="D9" s="17">
         <v>24.35</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="17">
         <v>22.84</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="17">
         <v>27.66</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="17">
         <v>24.2</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="17">
         <v>22.41</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="17">
         <v>24.3</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="Q9" s="43">
+      <c r="O9" s="40"/>
+      <c r="Q9" s="35">
         <v>27.66</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="25">
+      <c r="R9" s="38">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="T9" s="35">
+        <v>29.76</v>
+      </c>
+      <c r="U9" s="46">
+        <v>28.64</v>
+      </c>
+      <c r="V9" s="38">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42"/>
+      <c r="C10" s="22">
         <v>20</v>
       </c>
       <c r="D10" s="17">
         <v>22.96</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="17">
         <v>21.55</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="17">
         <v>25.5</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="45" t="s">
         <v>61</v>
       </c>
       <c r="J10" s="17">
         <v>22.81</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="17">
         <v>21.44</v>
       </c>
-      <c r="M10" s="32"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="17">
         <v>22.34</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="Q10" s="43">
+      <c r="O10" s="40"/>
+      <c r="Q10" s="35">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="25">
+      <c r="R10" s="38">
+        <v>19</v>
+      </c>
+      <c r="T10" s="35">
+        <v>27.38</v>
+      </c>
+      <c r="U10" s="46">
+        <v>27.25</v>
+      </c>
+      <c r="V10" s="38">
+        <v>20.13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42"/>
+      <c r="C11" s="22">
         <v>25</v>
       </c>
       <c r="D11" s="17">
         <v>21.69</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17">
         <v>20.55</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="17">
         <v>24.45</v>
       </c>
-      <c r="I11" s="32"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="17">
         <v>21.6</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="17">
         <v>20.51</v>
       </c>
-      <c r="M11" s="32"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="17">
         <v>20.78</v>
       </c>
-      <c r="O11" s="35"/>
-      <c r="Q11" s="43">
+      <c r="O11" s="40"/>
+      <c r="Q11" s="35">
         <v>24.45</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20"/>
-      <c r="C12" s="25">
+      <c r="R11" s="38">
+        <v>18.04</v>
+      </c>
+      <c r="T11" s="35">
+        <v>26.3</v>
+      </c>
+      <c r="U11" s="46">
+        <v>25.99</v>
+      </c>
+      <c r="V11" s="38">
+        <v>19.149999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="22">
         <v>35</v>
       </c>
       <c r="D12" s="17">
         <v>19.62</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="17">
         <v>18.91</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="17">
         <v>21.35</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="28" t="s">
         <v>62</v>
       </c>
       <c r="J12" s="17">
         <v>19.57</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="17">
         <v>18.850000000000001</v>
       </c>
-      <c r="M12" s="32"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="17">
         <v>18.43</v>
       </c>
-      <c r="O12" s="35"/>
-      <c r="Q12" s="43">
+      <c r="O12" s="40"/>
+      <c r="Q12" s="35">
         <v>21.35</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+      <c r="R12" s="38">
+        <v>16.579999999999998</v>
+      </c>
+      <c r="T12" s="35">
+        <v>22.9</v>
+      </c>
+      <c r="U12" s="46">
+        <v>23.6</v>
+      </c>
+      <c r="V12" s="38">
+        <v>17.66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="M13" s="29"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M14" s="29"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="O6:O12"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="E5:E12"/>
+    <mergeCell ref="K5:K12"/>
     <mergeCell ref="G5:G12"/>
     <mergeCell ref="I5:I9"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="M8:M12"/>
     <mergeCell ref="M5:M6"/>
-    <mergeCell ref="O6:O12"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="E5:E12"/>
-    <mergeCell ref="K5:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2049,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8084B4-B9E0-491E-84E8-BB63FF77C291}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G12"/>
+    <sheetView topLeftCell="O3" zoomScale="78" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,370 +2301,478 @@
     <col min="33" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:22" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="44">
+      <c r="R4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="42"/>
+      <c r="C5" s="36">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D5" s="17">
         <v>26.78</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="44" t="s">
         <v>70</v>
       </c>
       <c r="F5" s="17">
         <v>25.18</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="44" t="s">
         <v>78</v>
       </c>
       <c r="H5" s="17">
         <v>31.03</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="17">
         <v>26.61</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="17">
         <v>23.8</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="44" t="s">
         <v>72</v>
       </c>
       <c r="N5" s="17">
         <v>30.4</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="Q5" s="35">
         <v>31.03</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="45">
+      <c r="R5" s="38">
+        <v>20.87</v>
+      </c>
+      <c r="T5" s="35">
+        <v>33.25</v>
+      </c>
+      <c r="U5" s="46">
+        <v>28.02</v>
+      </c>
+      <c r="V5" s="38">
+        <v>21.11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42"/>
+      <c r="C6" s="37">
         <v>0.05</v>
       </c>
       <c r="D6" s="17">
         <v>24.88</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="17">
         <v>23</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17">
         <v>30.6</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="17">
         <v>24.75</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="17">
         <v>22.72</v>
       </c>
-      <c r="M6" s="32"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="17">
         <v>26.76</v>
       </c>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="43">
+      <c r="O6" s="40"/>
+      <c r="Q6" s="35">
         <v>30.6</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="44">
+      <c r="R6" s="38">
+        <v>17.829999999999998</v>
+      </c>
+      <c r="T6" s="35">
+        <v>32.770000000000003</v>
+      </c>
+      <c r="U6" s="46">
+        <v>25.83</v>
+      </c>
+      <c r="V6" s="38">
+        <v>18.170000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="42"/>
+      <c r="C7" s="36">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D7" s="17">
         <v>23.5</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="17">
         <v>21.68</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="45" t="s">
         <v>79</v>
       </c>
       <c r="H7" s="17">
         <v>30.1</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="17">
         <v>23.74</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="K7" s="45" t="s">
         <v>61</v>
       </c>
       <c r="L7" s="17">
         <v>21.85</v>
       </c>
-      <c r="M7" s="32"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="17">
         <v>24.13</v>
       </c>
-      <c r="O7" s="42"/>
-      <c r="Q7" s="43">
+      <c r="O7" s="40"/>
+      <c r="Q7" s="35">
         <v>30.1</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="45">
+      <c r="R7" s="38">
+        <v>16.11</v>
+      </c>
+      <c r="T7" s="35">
+        <v>32.380000000000003</v>
+      </c>
+      <c r="U7" s="46">
+        <v>24.1</v>
+      </c>
+      <c r="V7" s="38">
+        <v>16.36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="37">
         <v>0.1</v>
       </c>
       <c r="D8" s="17">
         <v>22.42</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="17">
         <v>20.79</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="17">
         <v>29.37</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="17">
         <v>23.05</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="17">
         <v>21.09</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="45" t="s">
         <v>73</v>
       </c>
       <c r="N8" s="17">
         <v>22.14</v>
       </c>
-      <c r="O8" s="42"/>
-      <c r="Q8" s="43">
+      <c r="O8" s="40"/>
+      <c r="Q8" s="35">
         <v>29.37</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="45">
+      <c r="R8" s="38">
+        <v>14.82</v>
+      </c>
+      <c r="T8" s="35">
+        <v>31.36</v>
+      </c>
+      <c r="U8" s="46">
+        <v>22.73</v>
+      </c>
+      <c r="V8" s="38">
+        <v>15.11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
+      <c r="C9" s="37">
         <v>0.15</v>
       </c>
       <c r="D9" s="17">
         <v>20.68</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="17">
         <v>19.510000000000002</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="28" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="17">
         <v>27.92</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="17">
         <v>21.75</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="17">
         <v>19.77</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="17">
         <v>19.079999999999998</v>
       </c>
-      <c r="O9" s="42"/>
-      <c r="Q9" s="43">
+      <c r="O9" s="40"/>
+      <c r="Q9" s="35">
         <v>27.92</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="45">
+      <c r="R9" s="38">
+        <v>13.07</v>
+      </c>
+      <c r="T9" s="35">
+        <v>29.76</v>
+      </c>
+      <c r="U9" s="46">
+        <v>20.37</v>
+      </c>
+      <c r="V9" s="38">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42"/>
+      <c r="C10" s="37">
         <v>0.2</v>
       </c>
       <c r="D10" s="17">
         <v>19.37</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="17">
         <v>18.41</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="45" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="17">
         <v>26.06</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="17">
         <v>20.66</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="45" t="s">
         <v>71</v>
       </c>
       <c r="L10" s="17">
         <v>18.649999999999999</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="45" t="s">
         <v>74</v>
       </c>
       <c r="N10" s="17">
         <v>16.899999999999999</v>
       </c>
-      <c r="O10" s="42"/>
-      <c r="Q10" s="43">
+      <c r="O10" s="40"/>
+      <c r="Q10" s="35">
         <v>26.06</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="45">
+      <c r="R10" s="38">
+        <v>11.82</v>
+      </c>
+      <c r="T10" s="35">
+        <v>27.68</v>
+      </c>
+      <c r="U10" s="46">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="V10" s="38">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42"/>
+      <c r="C11" s="37">
         <v>0.25</v>
       </c>
       <c r="D11" s="17">
         <v>18.21</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17">
         <v>17.05</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="17">
         <v>24.61</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="45" t="s">
         <v>61</v>
       </c>
       <c r="J11" s="17">
         <v>19.760000000000002</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="17">
         <v>17.18</v>
       </c>
-      <c r="M11" s="32"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="17">
         <v>15.23</v>
       </c>
-      <c r="O11" s="42"/>
-      <c r="Q11" s="43">
+      <c r="O11" s="40"/>
+      <c r="Q11" s="35">
         <v>24.61</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20"/>
-      <c r="C12" s="45">
+      <c r="R11" s="38">
+        <v>10.86</v>
+      </c>
+      <c r="T11" s="35">
+        <v>26.39</v>
+      </c>
+      <c r="U11" s="46">
+        <v>17.11</v>
+      </c>
+      <c r="V11" s="38">
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="37">
         <v>0.35</v>
       </c>
       <c r="D12" s="17">
         <v>16.41</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="17">
         <v>14.82</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="17">
         <v>23.33</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="17">
         <v>18.059999999999999</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="17">
         <v>16.100000000000001</v>
       </c>
-      <c r="M12" s="32"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="17">
         <v>12.74</v>
       </c>
-      <c r="O12" s="42"/>
-      <c r="Q12" s="43">
+      <c r="O12" s="40"/>
+      <c r="Q12" s="35">
         <v>23.33</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+      <c r="R12" s="38">
+        <v>9.4</v>
+      </c>
+      <c r="T12" s="35">
+        <v>24.55</v>
+      </c>
+      <c r="U12" s="46">
+        <v>14.93</v>
+      </c>
+      <c r="V12" s="38">
+        <v>9.7200000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="M13" s="29"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M14" s="29"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="O5:O12"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="I5:I10"/>
+    <mergeCell ref="I11:I12"/>
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="M5:M7"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="M10:M12"/>
-    <mergeCell ref="O5:O12"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="E5:E12"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="I5:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="E5:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2434,10 +2780,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0264D35E-F6B5-4ED6-B341-9F6509165BBE}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="O2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,347 +2794,455 @@
     <col min="33" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:22" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="25">
+      <c r="R4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="42"/>
+      <c r="C5" s="22">
         <v>2.5</v>
       </c>
       <c r="D5" s="17">
         <v>29.82</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="44" t="s">
         <v>76</v>
       </c>
       <c r="F5" s="17">
         <v>29.01</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="44" t="s">
         <v>77</v>
       </c>
       <c r="H5" s="17">
         <v>30.52</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="17">
         <v>29.36</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="44" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="17">
         <v>39.049999999999997</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="44" t="s">
         <v>82</v>
       </c>
       <c r="N5" s="17">
         <v>37.520000000000003</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="32">
         <v>39.049999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="25">
+      <c r="R5" s="38">
+        <v>38.85</v>
+      </c>
+      <c r="T5" s="32">
+        <v>38.93</v>
+      </c>
+      <c r="U5" s="46">
+        <v>34.51</v>
+      </c>
+      <c r="V5" s="38">
+        <v>38.71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42"/>
+      <c r="C6" s="22">
         <v>5</v>
       </c>
       <c r="D6" s="17">
         <v>28.55</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="17">
         <v>27.88</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17">
         <v>29.02</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="17">
         <v>28.19</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="17">
         <v>33.64</v>
       </c>
-      <c r="M6" s="32"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="17">
         <v>33.130000000000003</v>
       </c>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="38">
+      <c r="O6" s="40"/>
+      <c r="Q6" s="32">
         <v>33.64</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="25">
+      <c r="R6" s="38">
+        <v>33.51</v>
+      </c>
+      <c r="T6" s="32">
+        <v>33.51</v>
+      </c>
+      <c r="U6" s="46">
+        <v>31.88</v>
+      </c>
+      <c r="V6" s="38">
+        <v>33.369999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="42"/>
+      <c r="C7" s="22">
         <v>7.5</v>
       </c>
       <c r="D7" s="17">
         <v>27.16</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="17">
         <v>26.62</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="17">
         <v>27.47</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="17">
         <v>26.88</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="17">
         <v>30.34</v>
       </c>
-      <c r="M7" s="32"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="17">
         <v>30.09</v>
       </c>
-      <c r="O7" s="42"/>
-      <c r="Q7" s="38">
+      <c r="O7" s="40"/>
+      <c r="Q7" s="32">
         <v>30.34</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="25">
+      <c r="R7" s="38">
+        <v>30.25</v>
+      </c>
+      <c r="T7" s="32">
+        <v>30.19</v>
+      </c>
+      <c r="U7" s="46">
+        <v>29.45</v>
+      </c>
+      <c r="V7" s="38">
+        <v>30.09</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="22">
         <v>10</v>
       </c>
       <c r="D8" s="17">
         <v>25.82</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="17">
         <v>23.66</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="17">
         <v>26.02</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="17">
         <v>25.61</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="17">
         <v>27.97</v>
       </c>
-      <c r="M8" s="32"/>
+      <c r="M8" s="45"/>
       <c r="N8" s="17">
         <v>27.82</v>
       </c>
-      <c r="O8" s="42"/>
-      <c r="Q8" s="38">
+      <c r="O8" s="40"/>
+      <c r="Q8" s="32">
         <v>27.97</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="25">
+      <c r="R8" s="38">
+        <v>27.9</v>
+      </c>
+      <c r="T8" s="32">
+        <v>27.81</v>
+      </c>
+      <c r="U8" s="46">
+        <v>27.44</v>
+      </c>
+      <c r="V8" s="38">
+        <v>27.72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
+      <c r="C9" s="22">
         <v>15</v>
       </c>
       <c r="D9" s="17">
         <v>23.45</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="17">
         <v>23.17</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="17">
         <v>23.54</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="17">
         <v>23.31</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="17">
         <v>24.59</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="17">
         <v>24.51</v>
       </c>
-      <c r="O9" s="42"/>
-      <c r="Q9" s="38">
+      <c r="O9" s="40"/>
+      <c r="Q9" s="32">
         <v>24.59</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="25">
+      <c r="R9" s="38">
+        <v>24.53</v>
+      </c>
+      <c r="T9" s="32">
+        <v>24.4</v>
+      </c>
+      <c r="U9" s="46">
+        <v>24.27</v>
+      </c>
+      <c r="V9" s="38">
+        <v>24.34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42"/>
+      <c r="C10" s="22">
         <v>20</v>
       </c>
       <c r="D10" s="17">
         <v>21.49</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="17">
         <v>21.3</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="17">
         <v>21.53</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="17">
         <v>21.4</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="17">
         <v>22.17</v>
       </c>
-      <c r="M10" s="32"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="17">
         <v>22.13</v>
       </c>
-      <c r="O10" s="42"/>
-      <c r="Q10" s="38">
+      <c r="O10" s="40"/>
+      <c r="Q10" s="32">
         <v>22.17</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="25">
+      <c r="R10" s="38">
+        <v>22.13</v>
+      </c>
+      <c r="T10" s="32">
+        <v>21.95</v>
+      </c>
+      <c r="U10" s="46">
+        <v>21.9</v>
+      </c>
+      <c r="V10" s="38">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42"/>
+      <c r="C11" s="22">
         <v>25</v>
       </c>
       <c r="D11" s="17">
         <v>19.850000000000001</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17">
         <v>19.71</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="17">
         <v>19.86</v>
       </c>
-      <c r="I11" s="32"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="17">
         <v>19.79</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="17">
         <v>20.3</v>
       </c>
-      <c r="M11" s="32"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="17">
         <v>20.27</v>
       </c>
-      <c r="O11" s="42"/>
-      <c r="Q11" s="38">
+      <c r="O11" s="40"/>
+      <c r="Q11" s="32">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20"/>
-      <c r="C12" s="25">
+      <c r="R11" s="38">
+        <v>20.27</v>
+      </c>
+      <c r="T11" s="32">
+        <v>20.04</v>
+      </c>
+      <c r="U11" s="46">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="V11" s="38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="22">
         <v>35</v>
       </c>
       <c r="D12" s="17">
         <v>17.27</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="17">
         <v>17.190000000000001</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="17">
         <v>17.25</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="17">
         <v>17.239999999999998</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="17">
         <v>17.510000000000002</v>
       </c>
-      <c r="M12" s="32"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="17">
         <v>17.48</v>
       </c>
-      <c r="O12" s="42"/>
-      <c r="Q12" s="38">
+      <c r="O12" s="40"/>
+      <c r="Q12" s="32">
         <v>17.510000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+      <c r="R12" s="38">
+        <v>17.48</v>
+      </c>
+      <c r="T12" s="32">
+        <v>17.16</v>
+      </c>
+      <c r="U12" s="46">
+        <v>17.14</v>
+      </c>
+      <c r="V12" s="38">
+        <v>17.13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="M13" s="29"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M14" s="29"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="G5:G12"/>
-    <mergeCell ref="I5:I12"/>
-    <mergeCell ref="K5:K12"/>
     <mergeCell ref="M5:M12"/>
     <mergeCell ref="O5:O12"/>
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="E5:E12"/>
+    <mergeCell ref="G5:G12"/>
+    <mergeCell ref="I5:I12"/>
+    <mergeCell ref="K5:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2796,10 +3250,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7B3A6-323C-4763-8EC3-8A24B161C106}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="N1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2810,356 +3264,464 @@
     <col min="33" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:22" s="16" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="25">
+      <c r="R4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="42"/>
+      <c r="C5" s="22">
         <v>2.5</v>
       </c>
       <c r="D5" s="17">
         <v>30.17</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="44" t="s">
         <v>86</v>
       </c>
       <c r="F5" s="17">
         <v>29.54</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="44" t="s">
         <v>78</v>
       </c>
       <c r="H5" s="17">
         <v>31.28</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>87</v>
       </c>
       <c r="J5" s="17">
         <v>29.92</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="44" t="s">
         <v>88</v>
       </c>
       <c r="L5" s="17">
         <v>45.18</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="44" t="s">
         <v>89</v>
       </c>
       <c r="N5" s="17">
         <v>41.37</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="32">
         <v>45.18</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="25">
+      <c r="R5" s="38">
+        <v>45.19</v>
+      </c>
+      <c r="T5" s="32">
+        <v>45.12</v>
+      </c>
+      <c r="U5" s="46">
+        <v>35.94</v>
+      </c>
+      <c r="V5" s="38">
+        <v>45.12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42"/>
+      <c r="C6" s="22">
         <v>5</v>
       </c>
       <c r="D6" s="17">
         <v>30.06</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="17">
         <v>29.3</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17">
         <v>30.95</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="17">
         <v>29.82</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="17">
         <v>38.21</v>
       </c>
-      <c r="M6" s="32"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="17">
         <v>37.520000000000003</v>
       </c>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="38">
+      <c r="O6" s="40"/>
+      <c r="Q6" s="32">
         <v>38.21</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="25">
+      <c r="R6" s="38">
+        <v>38.21</v>
+      </c>
+      <c r="T6" s="32">
+        <v>38.119999999999997</v>
+      </c>
+      <c r="U6" s="46">
+        <v>35.25</v>
+      </c>
+      <c r="V6" s="38">
+        <v>38.119999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="42"/>
+      <c r="C7" s="22">
         <v>7.5</v>
       </c>
       <c r="D7" s="17">
         <v>29.96</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="17">
         <v>29.11</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="17">
         <v>30.66</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="17">
         <v>29.72</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="17">
         <v>35.51</v>
       </c>
-      <c r="M7" s="32"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="17">
         <v>35.369999999999997</v>
       </c>
-      <c r="O7" s="42"/>
-      <c r="Q7" s="38">
+      <c r="O7" s="40"/>
+      <c r="Q7" s="32">
         <v>35.51</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="25">
+      <c r="R7" s="38">
+        <v>35.51</v>
+      </c>
+      <c r="T7" s="32">
+        <v>35.43</v>
+      </c>
+      <c r="U7" s="46">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="V7" s="38">
+        <v>35.43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="22">
         <v>10</v>
       </c>
       <c r="D8" s="17">
         <v>29.76</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="17">
         <v>28.8</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="17">
         <v>30.15</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="17">
         <v>29.53</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="17">
         <v>32.590000000000003</v>
       </c>
-      <c r="M8" s="32"/>
+      <c r="M8" s="45"/>
       <c r="N8" s="17">
         <v>33.18</v>
       </c>
-      <c r="O8" s="46" t="s">
+      <c r="O8" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="33">
         <v>33.18</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="25">
+      <c r="R8" s="38">
+        <v>32.590000000000003</v>
+      </c>
+      <c r="T8" s="33">
+        <v>34.229999999999997</v>
+      </c>
+      <c r="U8" s="46">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="V8" s="38">
+        <v>32.479999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42"/>
+      <c r="C9" s="22">
         <v>15</v>
       </c>
       <c r="D9" s="17">
         <v>29.35</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="17">
         <v>28.24</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="17">
         <v>29.27</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="17">
         <v>29.15</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="17">
         <v>29.24</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="17">
         <v>31.12</v>
       </c>
-      <c r="O9" s="46" t="s">
+      <c r="O9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="33">
         <v>31.12</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="25">
+      <c r="R9" s="38">
+        <v>29.24</v>
+      </c>
+      <c r="T9" s="33">
+        <v>32.31</v>
+      </c>
+      <c r="U9" s="46">
+        <v>32.67</v>
+      </c>
+      <c r="V9" s="38">
+        <v>29.12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42"/>
+      <c r="C10" s="22">
         <v>20</v>
       </c>
       <c r="D10" s="17">
         <v>28.88</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="17">
         <v>27.61</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="17">
         <v>28.27</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="17">
         <v>28.69</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="17">
         <v>26.85</v>
       </c>
-      <c r="M10" s="32"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="17">
         <v>29.71</v>
       </c>
-      <c r="O10" s="42" t="s">
+      <c r="O10" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="33">
         <v>29.71</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="25">
+      <c r="R10" s="38">
+        <v>26.85</v>
+      </c>
+      <c r="T10" s="33">
+        <v>31.03</v>
+      </c>
+      <c r="U10" s="46">
+        <v>31.47</v>
+      </c>
+      <c r="V10" s="38">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42"/>
+      <c r="C11" s="22">
         <v>25</v>
       </c>
       <c r="D11" s="17">
         <v>28.35</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17">
         <v>26.96</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="17">
         <v>27.34</v>
       </c>
-      <c r="I11" s="32"/>
+      <c r="I11" s="45"/>
       <c r="J11" s="17">
         <v>28.19</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="17">
         <v>24.98</v>
       </c>
-      <c r="M11" s="32"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="17">
         <v>28.65</v>
       </c>
-      <c r="O11" s="42"/>
-      <c r="Q11" s="39">
+      <c r="O11" s="40"/>
+      <c r="Q11" s="33">
         <v>28.65</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20"/>
-      <c r="C12" s="25">
+      <c r="R11" s="38">
+        <v>24.98</v>
+      </c>
+      <c r="T11" s="33">
+        <v>29.76</v>
+      </c>
+      <c r="U11" s="46">
+        <v>30.3</v>
+      </c>
+      <c r="V11" s="38">
+        <v>24.84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="22">
         <v>35</v>
       </c>
       <c r="D12" s="17">
         <v>27.27</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="17">
         <v>25.64</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="17">
         <v>25.64</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="17">
         <v>27.14</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="17">
         <v>24.07</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M12" s="28" t="s">
         <v>65</v>
       </c>
       <c r="N12" s="17">
         <v>26.76</v>
       </c>
-      <c r="O12" s="42"/>
-      <c r="Q12" s="40">
+      <c r="O12" s="40"/>
+      <c r="Q12" s="34">
         <v>27.27</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+      <c r="R12" s="38">
+        <v>22.19</v>
+      </c>
+      <c r="T12" s="34">
+        <v>28.92</v>
+      </c>
+      <c r="U12" s="46">
+        <v>28.32</v>
+      </c>
+      <c r="V12" s="38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="M13" s="29"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M14" s="29"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G5:G12"/>
-    <mergeCell ref="I5:I12"/>
-    <mergeCell ref="K5:K12"/>
     <mergeCell ref="M5:M11"/>
     <mergeCell ref="O5:O7"/>
     <mergeCell ref="O10:O12"/>
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="E5:E12"/>
+    <mergeCell ref="G5:G12"/>
+    <mergeCell ref="I5:I12"/>
+    <mergeCell ref="K5:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>